<commit_message>
Inventaire + Kit montage modif
</commit_message>
<xml_diff>
--- a/06_Plateforme_Bron/Inventaire_Bron.xlsx
+++ b/06_Plateforme_Bron/Inventaire_Bron.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="150" windowWidth="13440" windowHeight="8310" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="150" windowWidth="13440" windowHeight="8310" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Regles_Nomenclature" sheetId="2" r:id="rId1"/>
     <sheet name="Visseurie" sheetId="1" r:id="rId2"/>
     <sheet name="Machines" sheetId="4" r:id="rId3"/>
+    <sheet name="Freinage" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">Machines!$2:$2</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="114">
   <si>
     <t>Liste d’inventaire</t>
   </si>
@@ -366,6 +367,12 @@
   </si>
   <si>
     <t>V_M8x60_8.8 + E_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scratsh anti dérapant </t>
+  </si>
+  <si>
+    <t>à coller sur les pédales</t>
   </si>
 </sst>
 </file>
@@ -938,6 +945,9 @@
     <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="7" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -947,9 +957,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="7" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="20 % - Accent1" xfId="24" builtinId="30" customBuiltin="1"/>
@@ -1000,7 +1007,7 @@
     <cellStyle name="Total" xfId="22" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="18" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="70">
     <dxf>
       <font>
         <strike val="0"/>
@@ -1308,6 +1315,344 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="11" formatCode="#,##0.00\ &quot;€&quot;;\-#,##0.00\ &quot;€&quot;"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1775,13 +2120,13 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="InventoryTable" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="InventoryTable" pivot="0" count="7">
-      <tableStyleElement type="wholeTable" dxfId="48"/>
-      <tableStyleElement type="headerRow" dxfId="47"/>
-      <tableStyleElement type="totalRow" dxfId="46"/>
-      <tableStyleElement type="firstColumn" dxfId="45"/>
-      <tableStyleElement type="lastColumn" dxfId="44"/>
-      <tableStyleElement type="firstRowStripe" dxfId="43"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="42"/>
+      <tableStyleElement type="wholeTable" dxfId="69"/>
+      <tableStyleElement type="headerRow" dxfId="68"/>
+      <tableStyleElement type="totalRow" dxfId="67"/>
+      <tableStyleElement type="firstColumn" dxfId="66"/>
+      <tableStyleElement type="lastColumn" dxfId="65"/>
+      <tableStyleElement type="firstRowStripe" dxfId="64"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="63"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1864,7 +2209,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="ListeInventaire" displayName="ListeInventaire" ref="A2:I82" headerRowDxfId="41" dataDxfId="40" totalsRowDxfId="39" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="ListeInventaire" displayName="ListeInventaire" ref="A2:I82" headerRowDxfId="62" dataDxfId="61" totalsRowDxfId="60" dataCellStyle="Normal">
+  <autoFilter ref="A2:I82"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Référence de stock" totalsRowLabel="Total" dataDxfId="59" totalsRowDxfId="58" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Nom" dataDxfId="57" totalsRowDxfId="56" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Description" dataDxfId="55" totalsRowDxfId="54" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Prix unitaire" totalsRowFunction="sum" dataDxfId="53" totalsRowDxfId="52" dataCellStyle="Monétaire"/>
+    <tableColumn id="5" name="Quantité en_x000a_stock" dataDxfId="51" totalsRowDxfId="50" dataCellStyle="Milliers"/>
+    <tableColumn id="6" name="Niveau de_x000a_réapprovisionnement" dataDxfId="49" totalsRowDxfId="48" dataCellStyle="Milliers"/>
+    <tableColumn id="7" name="Temps avant réapprovisionnement_x000a_en jours" dataDxfId="47" totalsRowDxfId="46" dataCellStyle="Milliers"/>
+    <tableColumn id="8" name="Quantité à réapprovisionner" dataDxfId="45" totalsRowDxfId="44" dataCellStyle="Milliers"/>
+    <tableColumn id="9" name="Retiré ?" totalsRowFunction="count" dataDxfId="43" totalsRowDxfId="42" dataCellStyle="Normal"/>
+  </tableColumns>
+  <tableStyleInfo name="InventoryTable" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{504A1905-F514-4f6f-8877-14C23A59335A}">
+      <x14:table altTextSummary="Entrez l’ID d’inventaire, le nom, la description, le prix unitaire, la quantité en stock, le seuil de réapprovisionnement, le temps avant réapprovisionnement en jours, la quantité à réapprovisionner et indiquez, par oui ou par non, si l’article est ou non encore disponible."/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="ListeInventaire3" displayName="ListeInventaire3" ref="A2:I82" headerRowDxfId="41" dataDxfId="40" totalsRowDxfId="39" dataCellStyle="Normal">
   <autoFilter ref="A2:I82"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Référence de stock" totalsRowLabel="Total" dataDxfId="38" totalsRowDxfId="37" dataCellStyle="Normal"/>
@@ -1886,8 +2254,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="ListeInventaire3" displayName="ListeInventaire3" ref="A2:I82" headerRowDxfId="20" dataDxfId="19" totalsRowDxfId="18" dataCellStyle="Normal">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="ListeInventaire34" displayName="ListeInventaire34" ref="A2:I82" headerRowDxfId="20" dataDxfId="19" totalsRowDxfId="18" dataCellStyle="Normal">
   <autoFilter ref="A2:I82"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Référence de stock" totalsRowLabel="Total" dataDxfId="16" totalsRowDxfId="17" dataCellStyle="Normal"/>
@@ -2316,17 +2684,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -2374,7 +2742,7 @@
     </row>
     <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="8"/>
@@ -2433,1195 +2801,1195 @@
       <c r="I7" s="8"/>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14" t="s">
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="12"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="9"/>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="12"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14" t="s">
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="12"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="9"/>
     </row>
     <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14" t="s">
+      <c r="C11" s="9"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="12"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="9"/>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14" t="s">
+      <c r="C12" s="9"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="12"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="9"/>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14" t="s">
+      <c r="C13" s="9"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="12"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="9"/>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12" t="s">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14" t="s">
+      <c r="D14" s="10"/>
+      <c r="E14" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="12"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="9"/>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12" t="s">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14" t="s">
+      <c r="C15" s="9"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="12"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="9"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="14" t="s">
+      <c r="C16" s="9"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="12"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="9"/>
     </row>
     <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12" t="s">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="14" t="s">
+      <c r="C17" s="9"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="12"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12" t="s">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="14" t="s">
+      <c r="D18" s="10"/>
+      <c r="E18" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="12"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="9"/>
     </row>
     <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12" t="s">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="14" t="s">
+      <c r="D19" s="10"/>
+      <c r="E19" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="12"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="9"/>
     </row>
     <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12" t="s">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="14" t="s">
+      <c r="C20" s="9"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="12"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="9"/>
     </row>
     <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12" t="s">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="14" t="s">
+      <c r="C21" s="9"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="12"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="9"/>
     </row>
     <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12" t="s">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="14" t="s">
+      <c r="C22" s="9"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="12"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="9"/>
     </row>
     <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12" t="s">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="14" t="s">
+      <c r="C23" s="9"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="12"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="9"/>
     </row>
     <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12" t="s">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="14" t="s">
+      <c r="C24" s="9"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="12"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="9"/>
     </row>
     <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12" t="s">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="14" t="s">
+      <c r="D25" s="10"/>
+      <c r="E25" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="12"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="9"/>
     </row>
     <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12" t="s">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="14" t="s">
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="12"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="9"/>
     </row>
     <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12" t="s">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="14" t="s">
+      <c r="C27" s="9"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="12"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="9"/>
     </row>
     <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12" t="s">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="14" t="s">
+      <c r="D28" s="10"/>
+      <c r="E28" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="12"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="9"/>
     </row>
     <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12" t="s">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="14" t="s">
+      <c r="D29" s="10"/>
+      <c r="E29" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="12"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="9"/>
     </row>
     <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12" t="s">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="14" t="s">
+      <c r="C30" s="9"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="12"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="9"/>
     </row>
     <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12" t="s">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="12"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="14" t="s">
+      <c r="C31" s="9"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="12"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="9"/>
     </row>
     <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12" t="s">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="14" t="s">
+      <c r="C32" s="9"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="12"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="9"/>
     </row>
     <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12" t="s">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="14" t="s">
+      <c r="D33" s="10"/>
+      <c r="E33" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="12"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="9"/>
     </row>
     <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12" t="s">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="14" t="s">
+      <c r="C34" s="9"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="12"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="9"/>
     </row>
     <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12" t="s">
+      <c r="A35" s="9"/>
+      <c r="B35" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="14" t="s">
+      <c r="C35" s="9"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="12"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="9"/>
     </row>
     <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12" t="s">
+      <c r="A36" s="9"/>
+      <c r="B36" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="14" t="s">
+      <c r="C36" s="9"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="12"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="9"/>
     </row>
     <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12" t="s">
+      <c r="A37" s="9"/>
+      <c r="B37" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="14" t="s">
+      <c r="C37" s="9"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="12"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="9"/>
     </row>
     <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12" t="s">
+      <c r="A38" s="9"/>
+      <c r="B38" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="14" t="s">
+      <c r="C38" s="9"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="12"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="9"/>
     </row>
     <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12" t="s">
+      <c r="A39" s="9"/>
+      <c r="B39" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C39" s="12"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="14" t="s">
+      <c r="C39" s="9"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="12"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="9"/>
     </row>
     <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12" t="s">
+      <c r="A40" s="9"/>
+      <c r="B40" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="14" t="s">
+      <c r="C40" s="9"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="12"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="9"/>
     </row>
     <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12" t="s">
+      <c r="A41" s="9"/>
+      <c r="B41" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C41" s="12"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="14" t="s">
+      <c r="C41" s="9"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="12"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="9"/>
     </row>
     <row r="42" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12" t="s">
+      <c r="A42" s="9"/>
+      <c r="B42" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="14" t="s">
+      <c r="C42" s="9"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="12"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="9"/>
     </row>
     <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12" t="s">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C43" s="12"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="14" t="s">
+      <c r="C43" s="9"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="12"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="9"/>
     </row>
     <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12" t="s">
+      <c r="A44" s="9"/>
+      <c r="B44" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="14" t="s">
+      <c r="C44" s="9"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="12"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="9"/>
     </row>
     <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12" t="s">
+      <c r="A45" s="9"/>
+      <c r="B45" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C45" s="12" t="s">
+      <c r="C45" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D45" s="13"/>
-      <c r="E45" s="14" t="s">
+      <c r="D45" s="10"/>
+      <c r="E45" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="12"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12" t="s">
+      <c r="A46" s="9"/>
+      <c r="B46" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D46" s="13"/>
-      <c r="E46" s="14" t="s">
+      <c r="D46" s="10"/>
+      <c r="E46" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="12"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="9"/>
     </row>
     <row r="47" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12" t="s">
+      <c r="A47" s="9"/>
+      <c r="B47" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C47" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D47" s="13"/>
-      <c r="E47" s="14" t="s">
+      <c r="D47" s="10"/>
+      <c r="E47" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="12"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="9"/>
     </row>
     <row r="48" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12" t="s">
+      <c r="A48" s="9"/>
+      <c r="B48" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C48" s="12" t="s">
+      <c r="C48" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D48" s="13"/>
-      <c r="E48" s="14" t="s">
+      <c r="D48" s="10"/>
+      <c r="E48" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="12"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="9"/>
     </row>
     <row r="49" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="12"/>
-      <c r="B49" s="12" t="s">
+      <c r="A49" s="9"/>
+      <c r="B49" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C49" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D49" s="13"/>
-      <c r="E49" s="14" t="s">
+      <c r="D49" s="10"/>
+      <c r="E49" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="12"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="9"/>
     </row>
     <row r="50" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="12"/>
-      <c r="B50" s="12" t="s">
+      <c r="A50" s="9"/>
+      <c r="B50" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C50" s="12" t="s">
+      <c r="C50" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D50" s="13"/>
-      <c r="E50" s="14" t="s">
+      <c r="D50" s="10"/>
+      <c r="E50" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="12"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="9"/>
     </row>
     <row r="51" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="12"/>
-      <c r="B51" s="12" t="s">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C51" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D51" s="13"/>
-      <c r="E51" s="14" t="s">
+      <c r="D51" s="10"/>
+      <c r="E51" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="12"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="9"/>
     </row>
     <row r="52" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="12"/>
-      <c r="B52" s="12" t="s">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C52" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D52" s="13"/>
-      <c r="E52" s="14" t="s">
+      <c r="D52" s="10"/>
+      <c r="E52" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="12"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="9"/>
     </row>
     <row r="53" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="12"/>
-      <c r="B53" s="12" t="s">
+      <c r="A53" s="9"/>
+      <c r="B53" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D53" s="13"/>
-      <c r="E53" s="14" t="s">
+      <c r="D53" s="10"/>
+      <c r="E53" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="12"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="9"/>
     </row>
     <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="12"/>
-      <c r="B54" s="12" t="s">
+      <c r="A54" s="9"/>
+      <c r="B54" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C54" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D54" s="13"/>
-      <c r="E54" s="14" t="s">
+      <c r="D54" s="10"/>
+      <c r="E54" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="12"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="9"/>
     </row>
     <row r="55" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="12"/>
-      <c r="B55" s="12" t="s">
+      <c r="A55" s="9"/>
+      <c r="B55" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="C55" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D55" s="13"/>
-      <c r="E55" s="14" t="s">
+      <c r="D55" s="10"/>
+      <c r="E55" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="12"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="9"/>
     </row>
     <row r="56" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="12"/>
-      <c r="B56" s="12" t="s">
+      <c r="A56" s="9"/>
+      <c r="B56" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C56" s="12" t="s">
+      <c r="C56" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D56" s="13"/>
-      <c r="E56" s="14" t="s">
+      <c r="D56" s="10"/>
+      <c r="E56" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="12"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="9"/>
     </row>
     <row r="57" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="12"/>
-      <c r="B57" s="12" t="s">
+      <c r="A57" s="9"/>
+      <c r="B57" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C57" s="12" t="s">
+      <c r="C57" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D57" s="13"/>
-      <c r="E57" s="14" t="s">
+      <c r="D57" s="10"/>
+      <c r="E57" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="12"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="9"/>
     </row>
     <row r="58" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="12"/>
-      <c r="B58" s="12" t="s">
+      <c r="A58" s="9"/>
+      <c r="B58" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C58" s="12" t="s">
+      <c r="C58" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D58" s="13"/>
-      <c r="E58" s="14" t="s">
+      <c r="D58" s="10"/>
+      <c r="E58" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="12"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="9"/>
     </row>
     <row r="59" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="12"/>
-      <c r="B59" s="12" t="s">
+      <c r="A59" s="9"/>
+      <c r="B59" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C59" s="12" t="s">
+      <c r="C59" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D59" s="13"/>
-      <c r="E59" s="14" t="s">
+      <c r="D59" s="10"/>
+      <c r="E59" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F59" s="14"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="12"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="9"/>
     </row>
     <row r="60" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="12"/>
-      <c r="B60" s="12" t="s">
+      <c r="A60" s="9"/>
+      <c r="B60" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C60" s="12" t="s">
+      <c r="C60" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D60" s="13"/>
-      <c r="E60" s="14" t="s">
+      <c r="D60" s="10"/>
+      <c r="E60" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="12"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="9"/>
     </row>
     <row r="61" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="12"/>
-      <c r="B61" s="12" t="s">
+      <c r="A61" s="9"/>
+      <c r="B61" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C61" s="12" t="s">
+      <c r="C61" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D61" s="13"/>
-      <c r="E61" s="14" t="s">
+      <c r="D61" s="10"/>
+      <c r="E61" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F61" s="14"/>
-      <c r="G61" s="14"/>
-      <c r="H61" s="14"/>
-      <c r="I61" s="12"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
+      <c r="I61" s="9"/>
     </row>
     <row r="62" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="12"/>
-      <c r="B62" s="12" t="s">
+      <c r="A62" s="9"/>
+      <c r="B62" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C62" s="12" t="s">
+      <c r="C62" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D62" s="13"/>
-      <c r="E62" s="14" t="s">
+      <c r="D62" s="10"/>
+      <c r="E62" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-      <c r="H62" s="14"/>
-      <c r="I62" s="12"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="9"/>
     </row>
     <row r="63" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="12"/>
-      <c r="B63" s="12" t="s">
+      <c r="A63" s="9"/>
+      <c r="B63" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C63" s="12"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="14" t="s">
+      <c r="C63" s="9"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="12"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="9"/>
     </row>
     <row r="64" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="12"/>
-      <c r="B64" s="12" t="s">
+      <c r="A64" s="9"/>
+      <c r="B64" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C64" s="12" t="s">
+      <c r="C64" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D64" s="13"/>
-      <c r="E64" s="14" t="s">
+      <c r="D64" s="10"/>
+      <c r="E64" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F64" s="14"/>
-      <c r="G64" s="14"/>
-      <c r="H64" s="14"/>
-      <c r="I64" s="12"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="9"/>
     </row>
     <row r="65" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="12"/>
-      <c r="B65" s="12" t="s">
+      <c r="A65" s="9"/>
+      <c r="B65" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C65" s="12"/>
-      <c r="D65" s="13"/>
-      <c r="E65" s="14" t="s">
+      <c r="C65" s="9"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="12"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="9"/>
     </row>
     <row r="66" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="12"/>
-      <c r="B66" s="12" t="s">
+      <c r="A66" s="9"/>
+      <c r="B66" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C66" s="12"/>
-      <c r="D66" s="13"/>
-      <c r="E66" s="14" t="s">
+      <c r="C66" s="9"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
-      <c r="I66" s="12"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="9"/>
     </row>
     <row r="67" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="12"/>
-      <c r="B67" s="12" t="s">
+      <c r="A67" s="9"/>
+      <c r="B67" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C67" s="12"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="14" t="s">
+      <c r="C67" s="9"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="12"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
+      <c r="I67" s="9"/>
     </row>
     <row r="68" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="12"/>
-      <c r="B68" s="12" t="s">
+      <c r="A68" s="9"/>
+      <c r="B68" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C68" s="12"/>
-      <c r="D68" s="13"/>
-      <c r="E68" s="14" t="s">
+      <c r="C68" s="9"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F68" s="14"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
-      <c r="I68" s="12"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="11"/>
+      <c r="I68" s="9"/>
     </row>
     <row r="69" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="12"/>
-      <c r="B69" s="12" t="s">
+      <c r="A69" s="9"/>
+      <c r="B69" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C69" s="12"/>
-      <c r="D69" s="13"/>
-      <c r="E69" s="14" t="s">
+      <c r="C69" s="9"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="F69" s="14"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14"/>
-      <c r="I69" s="12"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="11"/>
+      <c r="I69" s="9"/>
     </row>
     <row r="70" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="12"/>
-      <c r="B70" s="12" t="s">
+      <c r="A70" s="9"/>
+      <c r="B70" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C70" s="12"/>
-      <c r="D70" s="13"/>
-      <c r="E70" s="14" t="s">
+      <c r="C70" s="9"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F70" s="14"/>
-      <c r="G70" s="14"/>
-      <c r="H70" s="14"/>
-      <c r="I70" s="12"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
+      <c r="H70" s="11"/>
+      <c r="I70" s="9"/>
     </row>
     <row r="71" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="12"/>
-      <c r="B71" s="12" t="s">
+      <c r="A71" s="9"/>
+      <c r="B71" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C71" s="12"/>
-      <c r="D71" s="13"/>
-      <c r="E71" s="14" t="s">
+      <c r="C71" s="9"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F71" s="14"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="12"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
+      <c r="I71" s="9"/>
     </row>
     <row r="72" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="12"/>
-      <c r="B72" s="12" t="s">
+      <c r="A72" s="9"/>
+      <c r="B72" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C72" s="12"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="14" t="s">
+      <c r="C72" s="9"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F72" s="14"/>
-      <c r="G72" s="14"/>
-      <c r="H72" s="14"/>
-      <c r="I72" s="12"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="11"/>
+      <c r="I72" s="9"/>
     </row>
     <row r="73" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="12"/>
-      <c r="B73" s="12" t="s">
+      <c r="A73" s="9"/>
+      <c r="B73" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C73" s="12"/>
-      <c r="D73" s="13"/>
-      <c r="E73" s="14" t="s">
+      <c r="C73" s="9"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F73" s="14"/>
-      <c r="G73" s="14"/>
-      <c r="H73" s="14"/>
-      <c r="I73" s="12"/>
+      <c r="F73" s="11"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="11"/>
+      <c r="I73" s="9"/>
     </row>
     <row r="74" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="12"/>
-      <c r="B74" s="12" t="s">
+      <c r="A74" s="9"/>
+      <c r="B74" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C74" s="12"/>
-      <c r="D74" s="13"/>
-      <c r="E74" s="14" t="s">
+      <c r="C74" s="9"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F74" s="14"/>
-      <c r="G74" s="14"/>
-      <c r="H74" s="14"/>
-      <c r="I74" s="12"/>
+      <c r="F74" s="11"/>
+      <c r="G74" s="11"/>
+      <c r="H74" s="11"/>
+      <c r="I74" s="9"/>
     </row>
     <row r="75" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="12"/>
-      <c r="B75" s="12" t="s">
+      <c r="A75" s="9"/>
+      <c r="B75" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C75" s="12" t="s">
+      <c r="C75" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D75" s="13"/>
-      <c r="E75" s="14" t="s">
+      <c r="D75" s="10"/>
+      <c r="E75" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F75" s="14"/>
-      <c r="G75" s="14"/>
-      <c r="H75" s="14"/>
-      <c r="I75" s="12"/>
+      <c r="F75" s="11"/>
+      <c r="G75" s="11"/>
+      <c r="H75" s="11"/>
+      <c r="I75" s="9"/>
     </row>
     <row r="76" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="12"/>
-      <c r="B76" s="12" t="s">
+      <c r="A76" s="9"/>
+      <c r="B76" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C76" s="12" t="s">
+      <c r="C76" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D76" s="13"/>
-      <c r="E76" s="14" t="s">
+      <c r="D76" s="10"/>
+      <c r="E76" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="F76" s="14"/>
-      <c r="G76" s="14"/>
-      <c r="H76" s="14"/>
-      <c r="I76" s="12"/>
+      <c r="F76" s="11"/>
+      <c r="G76" s="11"/>
+      <c r="H76" s="11"/>
+      <c r="I76" s="9"/>
     </row>
     <row r="77" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="12"/>
-      <c r="B77" s="12" t="s">
+      <c r="A77" s="9"/>
+      <c r="B77" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C77" s="12"/>
-      <c r="D77" s="13"/>
-      <c r="E77" s="14" t="s">
+      <c r="C77" s="9"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="F77" s="14"/>
-      <c r="G77" s="14"/>
-      <c r="H77" s="14"/>
-      <c r="I77" s="12"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="11"/>
+      <c r="I77" s="9"/>
     </row>
     <row r="78" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="12"/>
-      <c r="B78" s="12" t="s">
+      <c r="A78" s="9"/>
+      <c r="B78" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C78" s="12" t="s">
+      <c r="C78" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D78" s="13"/>
-      <c r="E78" s="14" t="s">
+      <c r="D78" s="10"/>
+      <c r="E78" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F78" s="14"/>
-      <c r="G78" s="14"/>
-      <c r="H78" s="14"/>
-      <c r="I78" s="12"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="11"/>
+      <c r="I78" s="9"/>
     </row>
     <row r="79" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="12"/>
-      <c r="B79" s="12" t="s">
+      <c r="A79" s="9"/>
+      <c r="B79" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C79" s="12" t="s">
+      <c r="C79" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D79" s="13"/>
-      <c r="E79" s="14" t="s">
+      <c r="D79" s="10"/>
+      <c r="E79" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F79" s="14"/>
-      <c r="G79" s="14"/>
-      <c r="H79" s="14"/>
-      <c r="I79" s="12"/>
+      <c r="F79" s="11"/>
+      <c r="G79" s="11"/>
+      <c r="H79" s="11"/>
+      <c r="I79" s="9"/>
     </row>
     <row r="80" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="12"/>
-      <c r="B80" s="12" t="s">
+      <c r="A80" s="9"/>
+      <c r="B80" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C80" s="12" t="s">
+      <c r="C80" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D80" s="13"/>
-      <c r="E80" s="14" t="s">
+      <c r="D80" s="10"/>
+      <c r="E80" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="F80" s="14"/>
-      <c r="G80" s="14"/>
-      <c r="H80" s="14"/>
-      <c r="I80" s="12"/>
+      <c r="F80" s="11"/>
+      <c r="G80" s="11"/>
+      <c r="H80" s="11"/>
+      <c r="I80" s="9"/>
     </row>
     <row r="81" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="12"/>
-      <c r="B81" s="12" t="s">
+      <c r="A81" s="9"/>
+      <c r="B81" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C81" s="12" t="s">
+      <c r="C81" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D81" s="13"/>
-      <c r="E81" s="14" t="s">
+      <c r="D81" s="10"/>
+      <c r="E81" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="F81" s="14"/>
-      <c r="G81" s="14"/>
-      <c r="H81" s="14"/>
-      <c r="I81" s="12"/>
+      <c r="F81" s="11"/>
+      <c r="G81" s="11"/>
+      <c r="H81" s="11"/>
+      <c r="I81" s="9"/>
     </row>
     <row r="82" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="12"/>
-      <c r="B82" s="12" t="s">
+      <c r="A82" s="9"/>
+      <c r="B82" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C82" s="12" t="s">
+      <c r="C82" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D82" s="13"/>
-      <c r="E82" s="14">
+      <c r="D82" s="10"/>
+      <c r="E82" s="11">
         <v>43193</v>
       </c>
-      <c r="F82" s="14"/>
-      <c r="G82" s="14"/>
-      <c r="H82" s="14"/>
-      <c r="I82" s="12"/>
+      <c r="F82" s="11"/>
+      <c r="G82" s="11"/>
+      <c r="H82" s="11"/>
+      <c r="I82" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3660,9 +4028,9 @@
   </sheetPr>
   <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3679,17 +4047,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -3733,7 +4101,7 @@
     </row>
     <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
-      <c r="B4" s="12"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="8"/>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
@@ -3776,829 +4144,829 @@
       <c r="I7" s="8"/>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="12"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="9"/>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="12"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="12"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="9"/>
     </row>
     <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="12"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="9"/>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="12"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="9"/>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="12"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="9"/>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="12"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="9"/>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="12"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="9"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="12"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="9"/>
     </row>
     <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="12"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="12"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="9"/>
     </row>
     <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="12"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="9"/>
     </row>
     <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="12"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="9"/>
     </row>
     <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="12"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="9"/>
     </row>
     <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="12"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="9"/>
     </row>
     <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="12"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="9"/>
     </row>
     <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="12"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="9"/>
     </row>
     <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="12"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="9"/>
     </row>
     <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="12"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="9"/>
     </row>
     <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="12"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="9"/>
     </row>
     <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="12"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="9"/>
     </row>
     <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="12"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="9"/>
     </row>
     <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="12"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="9"/>
     </row>
     <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="12"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="9"/>
     </row>
     <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="12"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="9"/>
     </row>
     <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="12"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="9"/>
     </row>
     <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="12"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="9"/>
     </row>
     <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="12"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="9"/>
     </row>
     <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="12"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="9"/>
     </row>
     <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="12"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="9"/>
     </row>
     <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="12"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="9"/>
     </row>
     <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="12"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="9"/>
     </row>
     <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="12"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="9"/>
     </row>
     <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="12"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="9"/>
     </row>
     <row r="42" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="12"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="9"/>
     </row>
     <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="12"/>
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="9"/>
     </row>
     <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="12"/>
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="9"/>
     </row>
     <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="12"/>
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="12"/>
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="9"/>
     </row>
     <row r="47" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="12"/>
+      <c r="A47" s="9"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="9"/>
     </row>
     <row r="48" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="12"/>
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="9"/>
     </row>
     <row r="49" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="12"/>
-      <c r="B49" s="12"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="12"/>
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="9"/>
     </row>
     <row r="50" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="12"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="12"/>
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="9"/>
     </row>
     <row r="51" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="12"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="12"/>
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="9"/>
     </row>
     <row r="52" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="12"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="12"/>
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="9"/>
     </row>
     <row r="53" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="12"/>
-      <c r="B53" s="12"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="12"/>
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="9"/>
     </row>
     <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="12"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="12"/>
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="9"/>
     </row>
     <row r="55" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="12"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="12"/>
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="9"/>
     </row>
     <row r="56" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="12"/>
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="12"/>
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="9"/>
     </row>
     <row r="57" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="12"/>
-      <c r="B57" s="12"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="12"/>
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="9"/>
     </row>
     <row r="58" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="12"/>
-      <c r="B58" s="12"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="12"/>
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="9"/>
     </row>
     <row r="59" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="12"/>
-      <c r="B59" s="12"/>
-      <c r="C59" s="12"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="12"/>
+      <c r="A59" s="9"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="9"/>
     </row>
     <row r="60" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="12"/>
-      <c r="B60" s="12"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="13"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="12"/>
+      <c r="A60" s="9"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="9"/>
     </row>
     <row r="61" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="12"/>
-      <c r="B61" s="12"/>
-      <c r="C61" s="12"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="14"/>
-      <c r="G61" s="14"/>
-      <c r="H61" s="14"/>
-      <c r="I61" s="12"/>
+      <c r="A61" s="9"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
+      <c r="I61" s="9"/>
     </row>
     <row r="62" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="12"/>
-      <c r="B62" s="12"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="13"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-      <c r="H62" s="14"/>
-      <c r="I62" s="12"/>
+      <c r="A62" s="9"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="9"/>
     </row>
     <row r="63" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="12"/>
-      <c r="B63" s="12"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="12"/>
+      <c r="A63" s="9"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="9"/>
     </row>
     <row r="64" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="12"/>
-      <c r="B64" s="12"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="13"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="14"/>
-      <c r="G64" s="14"/>
-      <c r="H64" s="14"/>
-      <c r="I64" s="12"/>
+      <c r="A64" s="9"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="9"/>
     </row>
     <row r="65" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="12"/>
-      <c r="B65" s="12"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="13"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="12"/>
+      <c r="A65" s="9"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="9"/>
     </row>
     <row r="66" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="12"/>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="13"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
-      <c r="I66" s="12"/>
+      <c r="A66" s="9"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="9"/>
     </row>
     <row r="67" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="12"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="12"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="12"/>
+      <c r="A67" s="9"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
+      <c r="I67" s="9"/>
     </row>
     <row r="68" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="12"/>
-      <c r="B68" s="12"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="13"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
-      <c r="I68" s="12"/>
+      <c r="A68" s="9"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="11"/>
+      <c r="I68" s="9"/>
     </row>
     <row r="69" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="12"/>
-      <c r="B69" s="12"/>
-      <c r="C69" s="12"/>
-      <c r="D69" s="13"/>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14"/>
-      <c r="I69" s="12"/>
+      <c r="A69" s="9"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="11"/>
+      <c r="I69" s="9"/>
     </row>
     <row r="70" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="12"/>
-      <c r="B70" s="12"/>
-      <c r="C70" s="12"/>
-      <c r="D70" s="13"/>
-      <c r="E70" s="14"/>
-      <c r="F70" s="14"/>
-      <c r="G70" s="14"/>
-      <c r="H70" s="14"/>
-      <c r="I70" s="12"/>
+      <c r="A70" s="9"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
+      <c r="H70" s="11"/>
+      <c r="I70" s="9"/>
     </row>
     <row r="71" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="12"/>
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="13"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="12"/>
+      <c r="A71" s="9"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
+      <c r="I71" s="9"/>
     </row>
     <row r="72" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="12"/>
-      <c r="B72" s="12"/>
-      <c r="C72" s="12"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
-      <c r="G72" s="14"/>
-      <c r="H72" s="14"/>
-      <c r="I72" s="12"/>
+      <c r="A72" s="9"/>
+      <c r="B72" s="9"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="11"/>
+      <c r="I72" s="9"/>
     </row>
     <row r="73" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="12"/>
-      <c r="B73" s="12"/>
-      <c r="C73" s="12"/>
-      <c r="D73" s="13"/>
-      <c r="E73" s="14"/>
-      <c r="F73" s="14"/>
-      <c r="G73" s="14"/>
-      <c r="H73" s="14"/>
-      <c r="I73" s="12"/>
+      <c r="A73" s="9"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="11"/>
+      <c r="I73" s="9"/>
     </row>
     <row r="74" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="12"/>
-      <c r="B74" s="12"/>
-      <c r="C74" s="12"/>
-      <c r="D74" s="13"/>
-      <c r="E74" s="14"/>
-      <c r="F74" s="14"/>
-      <c r="G74" s="14"/>
-      <c r="H74" s="14"/>
-      <c r="I74" s="12"/>
+      <c r="A74" s="9"/>
+      <c r="B74" s="9"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="11"/>
+      <c r="F74" s="11"/>
+      <c r="G74" s="11"/>
+      <c r="H74" s="11"/>
+      <c r="I74" s="9"/>
     </row>
     <row r="75" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="12"/>
-      <c r="B75" s="12"/>
-      <c r="C75" s="12"/>
-      <c r="D75" s="13"/>
-      <c r="E75" s="14"/>
-      <c r="F75" s="14"/>
-      <c r="G75" s="14"/>
-      <c r="H75" s="14"/>
-      <c r="I75" s="12"/>
+      <c r="A75" s="9"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="11"/>
+      <c r="F75" s="11"/>
+      <c r="G75" s="11"/>
+      <c r="H75" s="11"/>
+      <c r="I75" s="9"/>
     </row>
     <row r="76" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="12"/>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="13"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="14"/>
-      <c r="G76" s="14"/>
-      <c r="H76" s="14"/>
-      <c r="I76" s="12"/>
+      <c r="A76" s="9"/>
+      <c r="B76" s="9"/>
+      <c r="C76" s="9"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
+      <c r="G76" s="11"/>
+      <c r="H76" s="11"/>
+      <c r="I76" s="9"/>
     </row>
     <row r="77" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="12"/>
-      <c r="B77" s="12"/>
-      <c r="C77" s="12"/>
-      <c r="D77" s="13"/>
-      <c r="E77" s="14"/>
-      <c r="F77" s="14"/>
-      <c r="G77" s="14"/>
-      <c r="H77" s="14"/>
-      <c r="I77" s="12"/>
+      <c r="A77" s="9"/>
+      <c r="B77" s="9"/>
+      <c r="C77" s="9"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="11"/>
+      <c r="I77" s="9"/>
     </row>
     <row r="78" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="12"/>
-      <c r="B78" s="12"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="13"/>
-      <c r="E78" s="14"/>
-      <c r="F78" s="14"/>
-      <c r="G78" s="14"/>
-      <c r="H78" s="14"/>
-      <c r="I78" s="12"/>
+      <c r="A78" s="9"/>
+      <c r="B78" s="9"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="10"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="11"/>
+      <c r="I78" s="9"/>
     </row>
     <row r="79" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="12"/>
-      <c r="B79" s="12"/>
-      <c r="C79" s="12"/>
-      <c r="D79" s="13"/>
-      <c r="E79" s="14"/>
-      <c r="F79" s="14"/>
-      <c r="G79" s="14"/>
-      <c r="H79" s="14"/>
-      <c r="I79" s="12"/>
+      <c r="A79" s="9"/>
+      <c r="B79" s="9"/>
+      <c r="C79" s="9"/>
+      <c r="D79" s="10"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="11"/>
+      <c r="G79" s="11"/>
+      <c r="H79" s="11"/>
+      <c r="I79" s="9"/>
     </row>
     <row r="80" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="12"/>
-      <c r="B80" s="12"/>
-      <c r="C80" s="12"/>
-      <c r="D80" s="13"/>
-      <c r="E80" s="14"/>
-      <c r="F80" s="14"/>
-      <c r="G80" s="14"/>
-      <c r="H80" s="14"/>
-      <c r="I80" s="12"/>
+      <c r="A80" s="9"/>
+      <c r="B80" s="9"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="10"/>
+      <c r="E80" s="11"/>
+      <c r="F80" s="11"/>
+      <c r="G80" s="11"/>
+      <c r="H80" s="11"/>
+      <c r="I80" s="9"/>
     </row>
     <row r="81" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="12"/>
-      <c r="B81" s="12"/>
-      <c r="C81" s="12"/>
-      <c r="D81" s="13"/>
-      <c r="E81" s="14"/>
-      <c r="F81" s="14"/>
-      <c r="G81" s="14"/>
-      <c r="H81" s="14"/>
-      <c r="I81" s="12"/>
+      <c r="A81" s="9"/>
+      <c r="B81" s="9"/>
+      <c r="C81" s="9"/>
+      <c r="D81" s="10"/>
+      <c r="E81" s="11"/>
+      <c r="F81" s="11"/>
+      <c r="G81" s="11"/>
+      <c r="H81" s="11"/>
+      <c r="I81" s="9"/>
     </row>
     <row r="82" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="12"/>
-      <c r="B82" s="12"/>
-      <c r="C82" s="12"/>
-      <c r="D82" s="13"/>
-      <c r="E82" s="14"/>
-      <c r="F82" s="14"/>
-      <c r="G82" s="14"/>
-      <c r="H82" s="14"/>
-      <c r="I82" s="12"/>
+      <c r="A82" s="9"/>
+      <c r="B82" s="9"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="10"/>
+      <c r="E82" s="11"/>
+      <c r="F82" s="11"/>
+      <c r="G82" s="11"/>
+      <c r="H82" s="11"/>
+      <c r="I82" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4626,4 +4994,976 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I82"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="28.75" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.58203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.58203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="23.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.58203125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="14"/>
+    </row>
+    <row r="2" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
+      <c r="B3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
+      <c r="B5"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="9"/>
+    </row>
+    <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="9"/>
+    </row>
+    <row r="36" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="9"/>
+    </row>
+    <row r="37" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="9"/>
+    </row>
+    <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="9"/>
+    </row>
+    <row r="40" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="9"/>
+    </row>
+    <row r="41" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="9"/>
+    </row>
+    <row r="43" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="9"/>
+    </row>
+    <row r="44" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="9"/>
+    </row>
+    <row r="45" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="9"/>
+    </row>
+    <row r="46" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="9"/>
+    </row>
+    <row r="47" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="9"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="9"/>
+    </row>
+    <row r="48" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="9"/>
+    </row>
+    <row r="49" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="9"/>
+    </row>
+    <row r="50" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="9"/>
+    </row>
+    <row r="51" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="9"/>
+    </row>
+    <row r="52" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="9"/>
+    </row>
+    <row r="53" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="9"/>
+    </row>
+    <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="9"/>
+    </row>
+    <row r="55" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="9"/>
+    </row>
+    <row r="56" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="9"/>
+    </row>
+    <row r="57" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="9"/>
+    </row>
+    <row r="58" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="9"/>
+    </row>
+    <row r="59" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="9"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="9"/>
+    </row>
+    <row r="60" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="9"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="9"/>
+    </row>
+    <row r="61" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="9"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
+      <c r="I61" s="9"/>
+    </row>
+    <row r="62" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="9"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="9"/>
+    </row>
+    <row r="63" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="9"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="9"/>
+    </row>
+    <row r="64" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="9"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="9"/>
+    </row>
+    <row r="65" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="9"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="9"/>
+    </row>
+    <row r="66" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="9"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="9"/>
+    </row>
+    <row r="67" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="9"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
+      <c r="I67" s="9"/>
+    </row>
+    <row r="68" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="9"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="11"/>
+      <c r="I68" s="9"/>
+    </row>
+    <row r="69" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="9"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="11"/>
+      <c r="I69" s="9"/>
+    </row>
+    <row r="70" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="9"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
+      <c r="H70" s="11"/>
+      <c r="I70" s="9"/>
+    </row>
+    <row r="71" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="9"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
+      <c r="I71" s="9"/>
+    </row>
+    <row r="72" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="9"/>
+      <c r="B72" s="9"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="11"/>
+      <c r="I72" s="9"/>
+    </row>
+    <row r="73" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="9"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="11"/>
+      <c r="I73" s="9"/>
+    </row>
+    <row r="74" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="9"/>
+      <c r="B74" s="9"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="11"/>
+      <c r="F74" s="11"/>
+      <c r="G74" s="11"/>
+      <c r="H74" s="11"/>
+      <c r="I74" s="9"/>
+    </row>
+    <row r="75" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="9"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="11"/>
+      <c r="F75" s="11"/>
+      <c r="G75" s="11"/>
+      <c r="H75" s="11"/>
+      <c r="I75" s="9"/>
+    </row>
+    <row r="76" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="9"/>
+      <c r="B76" s="9"/>
+      <c r="C76" s="9"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
+      <c r="G76" s="11"/>
+      <c r="H76" s="11"/>
+      <c r="I76" s="9"/>
+    </row>
+    <row r="77" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="9"/>
+      <c r="B77" s="9"/>
+      <c r="C77" s="9"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="11"/>
+      <c r="I77" s="9"/>
+    </row>
+    <row r="78" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="9"/>
+      <c r="B78" s="9"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="10"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="11"/>
+      <c r="I78" s="9"/>
+    </row>
+    <row r="79" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="9"/>
+      <c r="B79" s="9"/>
+      <c r="C79" s="9"/>
+      <c r="D79" s="10"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="11"/>
+      <c r="G79" s="11"/>
+      <c r="H79" s="11"/>
+      <c r="I79" s="9"/>
+    </row>
+    <row r="80" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="9"/>
+      <c r="B80" s="9"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="10"/>
+      <c r="E80" s="11"/>
+      <c r="F80" s="11"/>
+      <c r="G80" s="11"/>
+      <c r="H80" s="11"/>
+      <c r="I80" s="9"/>
+    </row>
+    <row r="81" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="9"/>
+      <c r="B81" s="9"/>
+      <c r="C81" s="9"/>
+      <c r="D81" s="10"/>
+      <c r="E81" s="11"/>
+      <c r="F81" s="11"/>
+      <c r="G81" s="11"/>
+      <c r="H81" s="11"/>
+      <c r="I81" s="9"/>
+    </row>
+    <row r="82" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="9"/>
+      <c r="B82" s="9"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="10"/>
+      <c r="E82" s="11"/>
+      <c r="F82" s="11"/>
+      <c r="G82" s="11"/>
+      <c r="H82" s="11"/>
+      <c r="I82" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <dataValidations count="10">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Créez une liste d'inventaire dans cette feuille de calcul. Le titre de cette feuille de calcul figure dans cette cellule. Entrez les détails dans le tableau ci-dessous." sqref="A1:I1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Entrez l’ID d’inventaire dans cette colonne sous ce titre. Utilisez les filtres de titre pour trouver des entrées spécifiques" sqref="A2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Entrez le nom dans cette colonne sous ce titre." sqref="B2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Entrez la description dans cette colonne sous ce titre." sqref="C2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Entrez le prix unitaire dans cette colonne sous ce titre." sqref="D2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Entrez la quantité en stock dans cette colonne sous ce titre." sqref="E2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Entrez le seuil de réapprovisionnement dans cette colonne sous ce titre." sqref="F2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Entrez le temps avant réapprovisionnement exprimé en jours dans cette colonne sous ce titre." sqref="G2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Entrez la quantité à réapprovisionner dans cette colonne sous ce titre." sqref="H2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Indiquez si l’article n’est plus disponible dans cette colonne sous ce titre." sqref="I2"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
MAJ gantt et réorganisation avec ajout doc CNN FEM CATIA
</commit_message>
<xml_diff>
--- a/06_Plateforme_Bron/Inventaire_Bron.xlsx
+++ b/06_Plateforme_Bron/Inventaire_Bron.xlsx
@@ -8,8 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gameiro Nicolas\Documents\EPSA\Intergen\06_Plateforme_Bron\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="150" windowWidth="13440" windowHeight="8310" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="150" windowWidth="13440" windowHeight="8310"/>
   </bookViews>
   <sheets>
     <sheet name="Regles_Nomenclature" sheetId="2" r:id="rId1"/>
@@ -1010,20 +1011,6 @@
   <dxfs count="70">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1315,6 +1302,20 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2258,15 +2259,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="ListeInventaire34" displayName="ListeInventaire34" ref="A2:I82" headerRowDxfId="20" dataDxfId="19" totalsRowDxfId="18" dataCellStyle="Normal">
   <autoFilter ref="A2:I82"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Référence de stock" totalsRowLabel="Total" dataDxfId="16" totalsRowDxfId="17" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Nom" dataDxfId="14" totalsRowDxfId="15" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Description" dataDxfId="12" totalsRowDxfId="13" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Prix unitaire" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="11" dataCellStyle="Monétaire"/>
-    <tableColumn id="5" name="Quantité en_x000a_stock" dataDxfId="8" totalsRowDxfId="9" dataCellStyle="Milliers"/>
-    <tableColumn id="6" name="Niveau de_x000a_réapprovisionnement" dataDxfId="6" totalsRowDxfId="7" dataCellStyle="Milliers"/>
-    <tableColumn id="7" name="Temps avant réapprovisionnement_x000a_en jours" dataDxfId="4" totalsRowDxfId="5" dataCellStyle="Milliers"/>
-    <tableColumn id="8" name="Quantité à réapprovisionner" dataDxfId="2" totalsRowDxfId="3" dataCellStyle="Milliers"/>
-    <tableColumn id="9" name="Retiré ?" totalsRowFunction="count" dataDxfId="0" totalsRowDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Référence de stock" totalsRowLabel="Total" dataDxfId="17" totalsRowDxfId="16" dataCellStyle="Normal"/>
+    <tableColumn id="2" name="Nom" dataDxfId="15" totalsRowDxfId="14" dataCellStyle="Normal"/>
+    <tableColumn id="3" name="Description" dataDxfId="13" totalsRowDxfId="12" dataCellStyle="Normal"/>
+    <tableColumn id="4" name="Prix unitaire" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10" dataCellStyle="Monétaire"/>
+    <tableColumn id="5" name="Quantité en_x000a_stock" dataDxfId="9" totalsRowDxfId="8" dataCellStyle="Milliers"/>
+    <tableColumn id="6" name="Niveau de_x000a_réapprovisionnement" dataDxfId="7" totalsRowDxfId="6" dataCellStyle="Milliers"/>
+    <tableColumn id="7" name="Temps avant réapprovisionnement_x000a_en jours" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Milliers"/>
+    <tableColumn id="8" name="Quantité à réapprovisionner" dataDxfId="3" totalsRowDxfId="2" dataCellStyle="Milliers"/>
+    <tableColumn id="9" name="Retiré ?" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="InventoryTable" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2564,8 +2565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -5000,7 +5001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>

</xml_diff>